<commit_message>
added stats excel workbook + code to write to it from the other excel docs
</commit_message>
<xml_diff>
--- a/picks/Results.xlsx
+++ b/picks/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcoblin/SideProjects/WorldCup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcoblin/SideProjects/WorldCup/picks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12760" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="122">
   <si>
     <t>Name:</t>
   </si>
@@ -778,6 +778,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -788,24 +806,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1118,7 +1118,7 @@
   <dimension ref="A1:M148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1133,50 +1133,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="H3" s="52" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="H3" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="52"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="51"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="57"/>
       <c r="H4" s="3" t="s">
         <v>62</v>
       </c>
@@ -1193,13 +1193,13 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
       <c r="H6" s="3" t="s">
         <v>64</v>
       </c>
@@ -1228,9 +1228,9 @@
       <c r="A8" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" t="s">
         <v>47</v>
       </c>
@@ -1245,9 +1245,9 @@
       <c r="A9" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
       <c r="F9" t="s">
         <v>76</v>
       </c>
@@ -1307,28 +1307,28 @@
       <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="53"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H14" s="52" t="s">
+      <c r="H14" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="52"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
       <c r="H15" s="3" t="s">
         <v>62</v>
       </c>
@@ -1584,22 +1584,22 @@
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C38" s="53" t="s">
+      <c r="C38" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="53"/>
+      <c r="D38" s="49"/>
       <c r="E38" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="37" t="s">
@@ -1815,22 +1815,22 @@
       <c r="F62" s="19"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C63" s="53" t="s">
+      <c r="C63" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="53"/>
+      <c r="D63" s="49"/>
       <c r="E63" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="53" t="s">
+      <c r="A65" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="53"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="53"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
@@ -1978,7 +1978,9 @@
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
+      <c r="E77" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F77" s="47" t="s">
         <v>93</v>
       </c>
@@ -1989,7 +1991,9 @@
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
+      <c r="E78" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F78" s="47" t="s">
         <v>94</v>
       </c>
@@ -1999,7 +2003,9 @@
         <v>91</v>
       </c>
       <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
+      <c r="D79" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="E79" s="7"/>
       <c r="F79" s="47" t="s">
         <v>50</v>
@@ -2522,22 +2528,22 @@
       <c r="H117" s="11"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C118" s="53" t="s">
+      <c r="C118" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D118" s="53"/>
+      <c r="D118" s="49"/>
       <c r="E118" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A120" s="53" t="s">
+      <c r="A120" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B120" s="53"/>
-      <c r="C120" s="53"/>
-      <c r="D120" s="53"/>
-      <c r="E120" s="53"/>
+      <c r="B120" s="49"/>
+      <c r="C120" s="49"/>
+      <c r="D120" s="49"/>
+      <c r="E120" s="49"/>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="59" t="s">
@@ -2903,16 +2909,21 @@
       <c r="D146" s="11"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C148" s="53" t="s">
+      <c r="C148" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D148" s="53"/>
+      <c r="D148" s="49"/>
       <c r="E148" s="8">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="A120:E120"/>
     <mergeCell ref="C148:D148"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="C13:D13"/>
@@ -2929,11 +2940,6 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A121:F121"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="A120:E120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>